<commit_message>
Parallel Execution changes added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\IdeaProjects\Assignment03_22550072\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D2AB78-CD49-470D-85A6-6DAD2CAC2799}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194B73EE-12F5-4499-B390-BEA7D83B18B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Test" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Item to search</t>
   </si>
@@ -37,34 +36,19 @@
     <t>New with box</t>
   </si>
   <si>
-    <t>Item condition</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
+    <t>Assertion value</t>
+  </si>
+  <si>
+    <t>Test case</t>
+  </si>
+  <si>
+    <t>Test case 3 &amp; 5</t>
+  </si>
+  <si>
     <t>Selected Item: Khamrah by Lattafa 3.4 oz EDP Perfume Cologne Unisex New in Box</t>
-  </si>
-  <si>
-    <t>Assertion value</t>
-  </si>
-  <si>
-    <t>Test case</t>
-  </si>
-  <si>
-    <t>Test case 1</t>
-  </si>
-  <si>
-    <t>Test case 2</t>
-  </si>
-  <si>
-    <t>Test case 3</t>
   </si>
 </sst>
 </file>
@@ -393,15 +377,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.33203125"/>
     <col min="2" max="2" customWidth="true" width="14.5546875"/>
     <col min="3" max="3" customWidth="true" width="15.6640625"/>
     <col min="4" max="4" customWidth="true" width="26.21875"/>
@@ -409,91 +393,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680A7B16-5042-493A-936D-7B3C17E376C4}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="14.5546875"/>
-    <col min="2" max="2" customWidth="true" width="12.88671875"/>
-    <col min="3" max="3" customWidth="true" width="26.21875"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
-        <v>0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>1</v>
       </c>
       <c r="C2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>